<commit_message>
Updated for find_nodules testing for Jinyi Wu
</commit_message>
<xml_diff>
--- a/FindNodulesEvaluator_result/FindNodulesEvaluation.xlsx
+++ b/FindNodulesEvaluator_result/FindNodulesEvaluation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>patientid</t>
   </si>
@@ -22,40 +22,70 @@
     <t>nodule_count</t>
   </si>
   <si>
-    <t>1.2.840.113704.1.111.11124.1523833084.11</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.9472.1522212912.10</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.5864.1523920989.10</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.4584.1522540656.15</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.6212.1522745545.10</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.6448.1522546028.19</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.2820.1522213231.10</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.5636.1522745175.10</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.6824.1522372272.11</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.12588.1523920580.10</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.7548.1523662552.11</t>
-  </si>
-  <si>
-    <t>1.2.840.113704.1.111.10220.1522055675.10</t>
+    <t>1.2.124.113532.58911.5035.4019.20141215.133333.481773016</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20150506.75718.118465244</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20130328.135119.198716743</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20160122.80312.171663275</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20150811.75809.650440447</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20140806.111714.337137653</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20151009.80949.928046274</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20141209.113442.452775586</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20150310.80257.788238479</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20131008.135136.284807444</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20140218.84528.729795016</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20130904.100041.204413260</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20151124.142522.16651958</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20150703.80256.431550864</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20150814.133633.676724434</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20151117.153628.53745043</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20120607.150937.40303505</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20150624.151847.383960241</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20120202.75608.72071115</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20150825.80314.728238332</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20140623.81923.173797738</t>
+  </si>
+  <si>
+    <t>1.2.124.113532.58911.5035.4019.20151116.140711.46964064</t>
   </si>
 </sst>
 </file>
@@ -413,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -440,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -448,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -456,7 +486,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -464,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -472,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -480,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -488,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -496,7 +526,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -504,7 +534,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -512,7 +542,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -520,7 +550,87 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>